<commit_message>
Added expressive range for: 	- Koch Curve 	- Fractal (Binary) Tree
</commit_message>
<xml_diff>
--- a/Expressive Range.xlsx
+++ b/Expressive Range.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github Repositories\L-systems\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74C9A1A9-AD20-4062-B8D5-31B166FC4342}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E5746A4-3B97-42C3-9A48-7C6ED52C10E5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{219E70A5-3509-45B7-BE7C-477FE8214683}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{219E70A5-3509-45B7-BE7C-477FE8214683}"/>
   </bookViews>
   <sheets>
-    <sheet name="Fractal Plants" sheetId="1" r:id="rId1"/>
-    <sheet name="Sirepinski Triangles" sheetId="2" r:id="rId2"/>
+    <sheet name="Koch Curve" sheetId="4" r:id="rId1"/>
+    <sheet name="Fractal (Binary) Tree" sheetId="3" r:id="rId2"/>
+    <sheet name="Fractal Plant" sheetId="1" r:id="rId3"/>
+    <sheet name="Sirepinski Triangle" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="3">
   <si>
     <t xml:space="preserve">Recursion </t>
   </si>
@@ -119,6 +121,738 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="sv" sz="1800" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Dimensions over Recursions</a:t>
+            </a:r>
+            <a:endParaRPr lang="sv-SE" sz="1400" b="0" i="0" baseline="0">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="LID4096"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Koch Curve'!$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Width</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Koch Curve'!$B$3:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Koch Curve'!$D$3:$D$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="1">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>540</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1620</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4860</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14580</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>43740</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>131220</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>393660</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-A5E9-46E0-BA39-60FD7C9C8A25}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Koch Curve'!$F$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Height</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Koch Curve'!$B$3:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Koch Curve'!$F$3:$F$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>260</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2420</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7280</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>21860</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>65600</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>196820</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-A5E9-46E0-BA39-60FD7C9C8A25}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="479043584"/>
+        <c:axId val="479040960"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="0"/>
+                <c:order val="0"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Koch Curve'!$C$2</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent1"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:cat>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Koch Curve'!$B$3:$B$12</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="10"/>
+                      <c:pt idx="1">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>5</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>7</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>8</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Koch Curve'!$C$3:$C$12</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="10"/>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000000-A5E9-46E0-BA39-60FD7C9C8A25}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="2"/>
+                <c:order val="2"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Koch Curve'!$E$2</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent3"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:cat>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Koch Curve'!$B$3:$B$12</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="10"/>
+                      <c:pt idx="1">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>5</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>7</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>8</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Koch Curve'!$E$3:$E$12</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="10"/>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000002-A5E9-46E0-BA39-60FD7C9C8A25}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+          </c:ext>
+        </c:extLst>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="479043584"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="LID4096"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="479040960"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="479040960"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="LID4096"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="479043584"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="LID4096"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="LID4096"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="sv-SE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="sv-SE"/>
+              <a:t>Dimensions over Recursions</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -159,7 +893,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Fractal Plants'!$D$2</c:f>
+              <c:f>'Fractal (Binary) Tree'!$D$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -182,10 +916,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Fractal Plants'!$B$3:$B$13</c:f>
+              <c:f>'Fractal (Binary) Tree'!$B$3:$B$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
@@ -215,45 +949,93 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>17</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Fractal Plants'!$D$3:$D$13</c:f>
+              <c:f>'Fractal (Binary) Tree'!$D$3:$D$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="1">
-                  <c:v>16</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>70</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>179</c:v>
+                  <c:v>112</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>415</c:v>
+                  <c:v>242</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>928</c:v>
+                  <c:v>496</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1953</c:v>
+                  <c:v>1012</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3988</c:v>
+                  <c:v>2040</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8054</c:v>
+                  <c:v>4102</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>16196</c:v>
+                  <c:v>8220</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>32473</c:v>
+                  <c:v>16462</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>32941</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>65905</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>131826</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>263670</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>527350</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1054876</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2109532</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4217962</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -261,7 +1043,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-71E9-4289-A61B-5203E4A6A8A2}"/>
+              <c16:uniqueId val="{00000001-4BC1-443D-8E79-EBC553EFDC44}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -270,7 +1052,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Fractal Plants'!$F$2</c:f>
+              <c:f>'Fractal (Binary) Tree'!$F$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -293,7 +1075,717 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Fractal Plants'!$B$3:$B$13</c:f>
+              <c:f>'Fractal (Binary) Tree'!$B$3:$B$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>17</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Fractal (Binary) Tree'!$F$3:$F$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="1">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>137</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>282</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>568</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1146</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2300</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4611</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9230</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>18471</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>36951</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>73911</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>147830</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>295693</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>591436</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1182370</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2366113</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4734968</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-4BC1-443D-8E79-EBC553EFDC44}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="472351280"/>
+        <c:axId val="472350296"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="0"/>
+                <c:order val="0"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Fractal (Binary) Tree'!$C$2</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent1"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:cat>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Fractal (Binary) Tree'!$B$3:$B$21</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="19"/>
+                      <c:pt idx="1">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>5</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>7</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>8</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>9</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>10</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>11</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>12</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>13</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>14</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>15</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>16</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>17</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Fractal (Binary) Tree'!$C$3:$C$21</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="19"/>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000000-4BC1-443D-8E79-EBC553EFDC44}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="2"/>
+                <c:order val="2"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Fractal (Binary) Tree'!$E$2</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent3"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:cat>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Fractal (Binary) Tree'!$B$3:$B$21</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="19"/>
+                      <c:pt idx="1">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>5</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>7</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>8</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>9</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>10</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>11</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>12</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>13</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>14</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>15</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>16</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>17</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Fractal (Binary) Tree'!$E$3:$E$21</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="19"/>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000002-4BC1-443D-8E79-EBC553EFDC44}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+          </c:ext>
+        </c:extLst>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="472351280"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="LID4096"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="472350296"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="472350296"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="LID4096"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="472351280"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="LID4096"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="LID4096"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="sv-SE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="sv" sz="1800" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Dimensions over Recursions</a:t>
+            </a:r>
+            <a:endParaRPr lang="sv-SE" sz="1400" b="0" i="0" baseline="0">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="LID4096"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Fractal Plant'!$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Width</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Fractal Plant'!$B$3:$B$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -332,7 +1824,118 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Fractal Plants'!$F$3:$F$13</c:f>
+              <c:f>'Fractal Plant'!$D$3:$D$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>179</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>415</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>928</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1953</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3988</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8054</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>16196</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>32473</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-71E9-4289-A61B-5203E4A6A8A2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Fractal Plant'!$F$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Height</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Fractal Plant'!$B$3:$B$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Fractal Plant'!$F$3:$F$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -398,7 +2001,7 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>'Fractal Plants'!$C$2</c15:sqref>
+                          <c15:sqref>'Fractal Plant'!$C$2</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -424,7 +2027,7 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>'Fractal Plants'!$B$3:$B$13</c15:sqref>
+                          <c15:sqref>'Fractal Plant'!$B$3:$B$13</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -469,7 +2072,7 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>'Fractal Plants'!$C$3:$C$13</c15:sqref>
+                          <c15:sqref>'Fractal Plant'!$C$3:$C$13</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -496,7 +2099,7 @@
                     <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>'Fractal Plants'!$E$2</c15:sqref>
+                          <c15:sqref>'Fractal Plant'!$E$2</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -522,7 +2125,7 @@
                     <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>'Fractal Plants'!$B$3:$B$13</c15:sqref>
+                          <c15:sqref>'Fractal Plant'!$B$3:$B$13</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -567,7 +2170,7 @@
                     <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>'Fractal Plants'!$E$3:$E$13</c15:sqref>
+                          <c15:sqref>'Fractal Plant'!$E$3:$E$13</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -771,7 +2374,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="sv-SE"/>
@@ -786,6 +2389,50 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="sv" sz="1800" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Dimensions over Recursions</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-SE">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -798,13 +2445,27 @@
         <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
         <a:lstStyle/>
         <a:p>
-          <a:pPr>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
             <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
+                <a:sysClr val="windowText" lastClr="000000">
                   <a:lumMod val="65000"/>
                   <a:lumOff val="35000"/>
-                </a:schemeClr>
+                </a:sysClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -826,7 +2487,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Sirepinski Triangles'!$D$2</c:f>
+              <c:f>'Sirepinski Triangle'!$D$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -849,7 +2510,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Sirepinski Triangles'!$B$3:$B$16</c:f>
+              <c:f>'Sirepinski Triangle'!$B$3:$B$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
@@ -897,7 +2558,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sirepinski Triangles'!$D$3:$D$16</c:f>
+              <c:f>'Sirepinski Triangle'!$D$3:$D$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
@@ -955,7 +2616,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Sirepinski Triangles'!$F$2</c:f>
+              <c:f>'Sirepinski Triangle'!$F$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -978,7 +2639,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Sirepinski Triangles'!$B$3:$B$16</c:f>
+              <c:f>'Sirepinski Triangle'!$B$3:$B$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
@@ -1026,7 +2687,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sirepinski Triangles'!$F$3:$F$16</c:f>
+              <c:f>'Sirepinski Triangle'!$F$3:$F$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
@@ -1101,7 +2762,7 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>'Sirepinski Triangles'!$C$2</c15:sqref>
+                          <c15:sqref>'Sirepinski Triangle'!$C$2</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -1127,7 +2788,7 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>'Sirepinski Triangles'!$B$3:$B$16</c15:sqref>
+                          <c15:sqref>'Sirepinski Triangle'!$B$3:$B$16</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -1181,7 +2842,7 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>'Sirepinski Triangles'!$C$3:$C$16</c15:sqref>
+                          <c15:sqref>'Sirepinski Triangle'!$C$3:$C$16</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -1208,7 +2869,7 @@
                     <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>'Sirepinski Triangles'!$E$2</c15:sqref>
+                          <c15:sqref>'Sirepinski Triangle'!$E$2</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -1234,7 +2895,7 @@
                     <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>'Sirepinski Triangles'!$B$3:$B$16</c15:sqref>
+                          <c15:sqref>'Sirepinski Triangle'!$B$3:$B$16</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -1288,7 +2949,7 @@
                     <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>'Sirepinski Triangles'!$E$3:$E$16</c15:sqref>
+                          <c15:sqref>'Sirepinski Triangle'!$E$3:$E$16</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -1572,6 +3233,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -2604,7 +4345,1121 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Diagram 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{02B7173F-CBD2-421C-9E14-6A19B6DA380C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Diagram 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{41A6859A-3D00-4AA0-8B2E-BD4FA49D3E47}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -2645,7 +5500,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -2655,10 +5510,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>601980</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>175260</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2982,11 +5837,366 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C224F06-128B-4384-AE17-08C4A3B01D35}">
+  <dimension ref="B2:F12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R14" sqref="R14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="2" spans="2:6" ht="21" x14ac:dyDescent="0.4">
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>60</v>
+      </c>
+      <c r="F4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>180</v>
+      </c>
+      <c r="F5">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>540</v>
+      </c>
+      <c r="F6">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="D7">
+        <v>1620</v>
+      </c>
+      <c r="F7">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B8">
+        <v>4</v>
+      </c>
+      <c r="D8">
+        <v>4860</v>
+      </c>
+      <c r="F8">
+        <v>2420</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B9">
+        <v>5</v>
+      </c>
+      <c r="D9">
+        <v>14580</v>
+      </c>
+      <c r="F9">
+        <v>7280</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B10">
+        <v>6</v>
+      </c>
+      <c r="D10">
+        <v>43740</v>
+      </c>
+      <c r="F10">
+        <v>21860</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B11">
+        <v>7</v>
+      </c>
+      <c r="D11">
+        <v>131220</v>
+      </c>
+      <c r="F11">
+        <v>65600</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B12">
+        <v>8</v>
+      </c>
+      <c r="D12">
+        <v>393660</v>
+      </c>
+      <c r="F12">
+        <v>196820</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{319ACC34-2B91-4441-B700-B08DAF7D856D}">
+  <dimension ref="B2:F21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S15" sqref="S15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="2" spans="2:6" ht="21" x14ac:dyDescent="0.4">
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>15</v>
+      </c>
+      <c r="F4">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>49</v>
+      </c>
+      <c r="F5">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>112</v>
+      </c>
+      <c r="F6">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="D7">
+        <v>242</v>
+      </c>
+      <c r="F7">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B8">
+        <v>4</v>
+      </c>
+      <c r="D8">
+        <v>496</v>
+      </c>
+      <c r="F8">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B9">
+        <v>5</v>
+      </c>
+      <c r="D9">
+        <v>1012</v>
+      </c>
+      <c r="F9">
+        <v>1146</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B10">
+        <v>6</v>
+      </c>
+      <c r="D10">
+        <v>2040</v>
+      </c>
+      <c r="F10">
+        <v>2300</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B11">
+        <v>7</v>
+      </c>
+      <c r="D11">
+        <v>4102</v>
+      </c>
+      <c r="F11">
+        <v>4611</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B12">
+        <v>8</v>
+      </c>
+      <c r="D12">
+        <v>8220</v>
+      </c>
+      <c r="F12">
+        <v>9230</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B13">
+        <v>9</v>
+      </c>
+      <c r="D13">
+        <v>16462</v>
+      </c>
+      <c r="F13">
+        <v>18471</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B14">
+        <v>10</v>
+      </c>
+      <c r="D14">
+        <v>32941</v>
+      </c>
+      <c r="F14">
+        <v>36951</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B15">
+        <v>11</v>
+      </c>
+      <c r="D15">
+        <v>65905</v>
+      </c>
+      <c r="F15">
+        <v>73911</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B16">
+        <v>12</v>
+      </c>
+      <c r="D16">
+        <v>131826</v>
+      </c>
+      <c r="F16">
+        <v>147830</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B17">
+        <v>13</v>
+      </c>
+      <c r="D17">
+        <v>263670</v>
+      </c>
+      <c r="F17">
+        <v>295693</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B18">
+        <v>14</v>
+      </c>
+      <c r="D18">
+        <v>527350</v>
+      </c>
+      <c r="F18">
+        <v>591436</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B19">
+        <v>15</v>
+      </c>
+      <c r="D19">
+        <v>1054876</v>
+      </c>
+      <c r="F19">
+        <v>1182370</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B20">
+        <v>16</v>
+      </c>
+      <c r="D20">
+        <v>2109532</v>
+      </c>
+      <c r="F20">
+        <v>2366113</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B21">
+        <v>17</v>
+      </c>
+      <c r="D21">
+        <v>4217962</v>
+      </c>
+      <c r="F21">
+        <v>4734968</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1406070-4149-41DF-851A-43E87B36136C}">
   <dimension ref="B2:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="B2" sqref="B2:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3121,12 +6331,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B6748DC-EB72-423E-8B37-AD2A635E2796}">
   <dimension ref="B2:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>